<commit_message>
Benin: Add oncho prestop supervisor forms.
</commit_message>
<xml_diff>
--- a/ONCHO/Impact Assessments/Benin/bj_oncho_prestop_1_site.xlsx
+++ b/ONCHO/Impact Assessments/Benin/bj_oncho_prestop_1_site.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositories\WHO\dsa-forms\ONCHO\Impact Assessments\Benin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5EFA707-B863-4B8E-AFC9-3645798F06C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{973FAC6B-E9C0-4049-AF7C-EC46762D4F9D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -296,12 +296,6 @@
     <t>French</t>
   </si>
   <si>
-    <t>bj_oncho_prestop_1_site</t>
-  </si>
-  <si>
-    <t>Benin ONCHO Pre stop - 1. Formulaire Site</t>
-  </si>
-  <si>
     <t xml:space="preserve">allow_choice_duplicates </t>
   </si>
   <si>
@@ -708,6 +702,12 @@
   </si>
   <si>
     <t>regex(.,'^[0-9]{2}$') and . &gt; 9 and . &lt; 1000</t>
+  </si>
+  <si>
+    <t>bj_oncho_prestop_1_site_v2</t>
+  </si>
+  <si>
+    <t>Benin ONCHO Pre stop TDM - 1. Formulaire Site V2</t>
   </si>
 </sst>
 </file>
@@ -1176,7 +1176,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -1252,10 +1252,10 @@
       </c>
       <c r="E2" s="13"/>
       <c r="F2" s="14" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="H2" s="13"/>
       <c r="I2" s="13"/>
@@ -1316,7 +1316,7 @@
         <v>73</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C5" s="12" t="s">
         <v>38</v>
@@ -1356,7 +1356,7 @@
       </c>
       <c r="K6" s="13"/>
       <c r="L6" s="14" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="7" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1367,7 +1367,7 @@
         <v>48</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D7" s="16"/>
       <c r="E7" s="13"/>
@@ -1543,10 +1543,10 @@
         <v>51</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D2" s="23"/>
       <c r="E2" s="23"/>
@@ -1557,10 +1557,10 @@
         <v>51</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D3" s="23"/>
       <c r="E3" s="23"/>
@@ -1571,10 +1571,10 @@
         <v>51</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D4" s="23"/>
       <c r="E4" s="23"/>
@@ -1599,10 +1599,10 @@
         <v>51</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D6" s="23"/>
       <c r="E6" s="23"/>
@@ -1613,10 +1613,10 @@
         <v>51</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D7" s="23"/>
       <c r="E7" s="23"/>
@@ -1627,10 +1627,10 @@
         <v>51</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D8" s="23"/>
       <c r="E8" s="23"/>
@@ -1655,13 +1655,13 @@
         <v>20</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D10" s="23" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E10" s="23"/>
       <c r="F10" s="23"/>
@@ -1671,13 +1671,13 @@
         <v>20</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D11" s="23" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E11" s="23"/>
       <c r="F11" s="23"/>
@@ -1687,10 +1687,10 @@
         <v>20</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D12" s="23" t="s">
         <v>58</v>
@@ -1703,13 +1703,13 @@
         <v>20</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D13" s="23" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E13" s="23"/>
       <c r="F13" s="23"/>
@@ -1719,13 +1719,13 @@
         <v>20</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D14" s="23" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E14" s="23"/>
       <c r="F14" s="23"/>
@@ -1735,13 +1735,13 @@
         <v>20</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D15" s="23" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E15" s="23"/>
       <c r="F15" s="23"/>
@@ -1799,13 +1799,13 @@
         <v>20</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D19" s="23" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E19" s="23"/>
       <c r="F19" s="23"/>
@@ -1815,13 +1815,13 @@
         <v>20</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D20" s="23" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E20" s="23"/>
       <c r="F20" s="23"/>
@@ -1831,13 +1831,13 @@
         <v>20</v>
       </c>
       <c r="B21" s="14" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D21" s="23" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E21" s="23"/>
       <c r="F21" s="23"/>
@@ -1847,13 +1847,13 @@
         <v>20</v>
       </c>
       <c r="B22" s="14" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D22" s="23" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E22" s="23"/>
       <c r="F22" s="23"/>
@@ -1863,13 +1863,13 @@
         <v>20</v>
       </c>
       <c r="B23" s="14" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D23" s="23" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E23" s="23"/>
       <c r="F23" s="23"/>
@@ -1879,13 +1879,13 @@
         <v>20</v>
       </c>
       <c r="B24" s="14" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D24" s="23" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E24" s="23"/>
       <c r="F24" s="23"/>
@@ -1895,13 +1895,13 @@
         <v>20</v>
       </c>
       <c r="B25" s="14" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D25" s="23" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E25" s="23"/>
       <c r="F25" s="23"/>
@@ -1911,13 +1911,13 @@
         <v>20</v>
       </c>
       <c r="B26" s="14" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D26" s="23" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E26" s="23"/>
       <c r="F26" s="23"/>
@@ -1927,13 +1927,13 @@
         <v>20</v>
       </c>
       <c r="B27" s="14" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D27" s="23" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E27" s="23"/>
       <c r="F27" s="23"/>
@@ -1943,13 +1943,13 @@
         <v>20</v>
       </c>
       <c r="B28" s="14" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D28" s="23" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E28" s="23"/>
       <c r="F28" s="23"/>
@@ -1959,13 +1959,13 @@
         <v>20</v>
       </c>
       <c r="B29" s="14" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D29" s="23" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E29" s="23"/>
       <c r="F29" s="23"/>
@@ -1975,13 +1975,13 @@
         <v>20</v>
       </c>
       <c r="B30" s="14" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C30" s="14" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D30" s="23" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E30" s="23"/>
       <c r="F30" s="23"/>
@@ -1991,13 +1991,13 @@
         <v>20</v>
       </c>
       <c r="B31" s="14" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C31" s="14" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D31" s="23" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E31" s="23"/>
       <c r="F31" s="23"/>
@@ -2007,13 +2007,13 @@
         <v>20</v>
       </c>
       <c r="B32" s="14" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D32" s="23" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E32" s="23"/>
       <c r="F32" s="23"/>
@@ -2023,13 +2023,13 @@
         <v>20</v>
       </c>
       <c r="B33" s="14" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D33" s="23" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E33" s="23"/>
       <c r="F33" s="23"/>
@@ -2039,10 +2039,10 @@
         <v>20</v>
       </c>
       <c r="B34" s="14" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D34" s="23" t="s">
         <v>58</v>
@@ -2055,13 +2055,13 @@
         <v>20</v>
       </c>
       <c r="B35" s="14" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D35" s="23" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E35" s="23"/>
       <c r="F35" s="23"/>
@@ -2071,13 +2071,13 @@
         <v>20</v>
       </c>
       <c r="B36" s="14" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D36" s="23" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E36" s="23"/>
       <c r="F36" s="23"/>
@@ -2087,10 +2087,10 @@
         <v>20</v>
       </c>
       <c r="B37" s="14" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C37" s="14" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D37" s="23" t="s">
         <v>58</v>
@@ -2119,13 +2119,13 @@
         <v>20</v>
       </c>
       <c r="B39" s="14" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C39" s="14" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D39" s="23" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E39" s="23"/>
       <c r="F39" s="23"/>
@@ -2135,13 +2135,13 @@
         <v>20</v>
       </c>
       <c r="B40" s="14" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C40" s="14" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D40" s="23" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E40" s="23"/>
       <c r="F40" s="23"/>
@@ -2151,13 +2151,13 @@
         <v>20</v>
       </c>
       <c r="B41" s="14" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C41" s="14" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D41" s="23" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E41" s="23"/>
       <c r="F41" s="23"/>
@@ -2167,10 +2167,10 @@
         <v>20</v>
       </c>
       <c r="B42" s="14" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C42" s="14" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D42" s="23" t="s">
         <v>75</v>
@@ -2183,10 +2183,10 @@
         <v>20</v>
       </c>
       <c r="B43" s="14" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C43" s="14" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D43" s="23" t="s">
         <v>75</v>
@@ -2215,14 +2215,14 @@
         <v>72</v>
       </c>
       <c r="B45" s="14" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C45" s="14" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D45" s="23"/>
       <c r="E45" s="23" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F45" s="22"/>
     </row>
@@ -2231,14 +2231,14 @@
         <v>72</v>
       </c>
       <c r="B46" s="14" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C46" s="14" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D46" s="23"/>
       <c r="E46" s="23" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F46" s="22"/>
     </row>
@@ -2263,14 +2263,14 @@
         <v>72</v>
       </c>
       <c r="B48" s="14" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C48" s="14" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D48" s="23"/>
       <c r="E48" s="23" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F48" s="22"/>
     </row>
@@ -2279,14 +2279,14 @@
         <v>72</v>
       </c>
       <c r="B49" s="14" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C49" s="14" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D49" s="23"/>
       <c r="E49" s="23" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F49" s="22"/>
     </row>
@@ -2302,7 +2302,7 @@
       </c>
       <c r="D50" s="23"/>
       <c r="E50" s="23" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F50" s="22"/>
     </row>
@@ -2311,14 +2311,14 @@
         <v>72</v>
       </c>
       <c r="B51" s="14" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C51" s="14" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D51" s="23"/>
       <c r="E51" s="23" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F51" s="22"/>
     </row>
@@ -2327,14 +2327,14 @@
         <v>72</v>
       </c>
       <c r="B52" s="14" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C52" s="14" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D52" s="23"/>
       <c r="E52" s="23" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="F52" s="22"/>
     </row>
@@ -2343,14 +2343,14 @@
         <v>72</v>
       </c>
       <c r="B53" s="14" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C53" s="14" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D53" s="23"/>
       <c r="E53" s="23" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F53" s="22"/>
     </row>
@@ -2359,14 +2359,14 @@
         <v>72</v>
       </c>
       <c r="B54" s="14" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C54" s="14" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D54" s="23"/>
       <c r="E54" s="23" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F54" s="22"/>
     </row>
@@ -2375,14 +2375,14 @@
         <v>72</v>
       </c>
       <c r="B55" s="14" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C55" s="14" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D55" s="23"/>
       <c r="E55" s="23" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F55" s="22"/>
     </row>
@@ -2391,14 +2391,14 @@
         <v>72</v>
       </c>
       <c r="B56" s="14" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C56" s="14" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D56" s="23"/>
       <c r="E56" s="23" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F56" s="22"/>
     </row>
@@ -2439,14 +2439,14 @@
         <v>72</v>
       </c>
       <c r="B59" s="14" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C59" s="14" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D59" s="23"/>
       <c r="E59" s="23" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F59" s="22"/>
     </row>
@@ -2471,14 +2471,14 @@
         <v>72</v>
       </c>
       <c r="B61" s="14" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C61" s="14" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D61" s="23"/>
       <c r="E61" s="23" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F61" s="22"/>
     </row>
@@ -2503,14 +2503,14 @@
         <v>72</v>
       </c>
       <c r="B63" s="14" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C63" s="14" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D63" s="23"/>
       <c r="E63" s="23" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F63" s="22"/>
     </row>
@@ -2519,14 +2519,14 @@
         <v>72</v>
       </c>
       <c r="B64" s="14" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C64" s="14" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D64" s="23"/>
       <c r="E64" s="23" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F64" s="22"/>
     </row>
@@ -2535,14 +2535,14 @@
         <v>72</v>
       </c>
       <c r="B65" s="14" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C65" s="14" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D65" s="23"/>
       <c r="E65" s="23" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F65" s="22"/>
     </row>
@@ -2551,14 +2551,14 @@
         <v>72</v>
       </c>
       <c r="B66" s="14" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C66" s="14" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D66" s="23"/>
       <c r="E66" s="23" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F66" s="22"/>
     </row>
@@ -2583,14 +2583,14 @@
         <v>72</v>
       </c>
       <c r="B68" s="14" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C68" s="14" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D68" s="23"/>
       <c r="E68" s="23" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F68" s="22"/>
     </row>
@@ -2599,14 +2599,14 @@
         <v>72</v>
       </c>
       <c r="B69" s="14" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C69" s="14" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D69" s="23"/>
       <c r="E69" s="23" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F69" s="22"/>
     </row>
@@ -2615,14 +2615,14 @@
         <v>72</v>
       </c>
       <c r="B70" s="14" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C70" s="14" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D70" s="23"/>
       <c r="E70" s="23" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="F70" s="22"/>
     </row>
@@ -2631,14 +2631,14 @@
         <v>72</v>
       </c>
       <c r="B71" s="14" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C71" s="14" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D71" s="23"/>
       <c r="E71" s="23" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F71" s="22"/>
     </row>
@@ -2647,14 +2647,14 @@
         <v>72</v>
       </c>
       <c r="B72" s="14" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C72" s="14" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D72" s="23"/>
       <c r="E72" s="23" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="F72" s="22"/>
     </row>
@@ -2663,14 +2663,14 @@
         <v>72</v>
       </c>
       <c r="B73" s="14" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C73" s="14" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D73" s="23"/>
       <c r="E73" s="23" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="F73" s="22"/>
     </row>
@@ -2679,14 +2679,14 @@
         <v>72</v>
       </c>
       <c r="B74" s="14" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C74" s="14" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D74" s="23"/>
       <c r="E74" s="23" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="F74" s="22"/>
     </row>
@@ -2695,14 +2695,14 @@
         <v>72</v>
       </c>
       <c r="B75" s="14" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C75" s="14" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D75" s="23"/>
       <c r="E75" s="23" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F75" s="22"/>
     </row>
@@ -2711,14 +2711,14 @@
         <v>72</v>
       </c>
       <c r="B76" s="14" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C76" s="14" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D76" s="23"/>
       <c r="E76" s="23" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F76" s="22"/>
     </row>
@@ -2727,14 +2727,14 @@
         <v>72</v>
       </c>
       <c r="B77" s="14" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C77" s="14" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D77" s="23"/>
       <c r="E77" s="23" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F77" s="22"/>
     </row>
@@ -2743,14 +2743,14 @@
         <v>72</v>
       </c>
       <c r="B78" s="14" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C78" s="14" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D78" s="23"/>
       <c r="E78" s="23" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F78" s="22"/>
     </row>
@@ -2775,14 +2775,14 @@
         <v>72</v>
       </c>
       <c r="B80" s="14" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C80" s="14" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D80" s="23"/>
       <c r="E80" s="23" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="F80" s="22"/>
     </row>
@@ -2791,14 +2791,14 @@
         <v>72</v>
       </c>
       <c r="B81" s="14" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C81" s="14" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D81" s="23"/>
       <c r="E81" s="23" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="F81" s="22"/>
     </row>
@@ -2807,14 +2807,14 @@
         <v>72</v>
       </c>
       <c r="B82" s="14" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C82" s="14" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D82" s="23"/>
       <c r="E82" s="23" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F82" s="22"/>
     </row>
@@ -2823,14 +2823,14 @@
         <v>72</v>
       </c>
       <c r="B83" s="14" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C83" s="14" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D83" s="23"/>
       <c r="E83" s="23" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="F83" s="22"/>
     </row>
@@ -2839,14 +2839,14 @@
         <v>72</v>
       </c>
       <c r="B84" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C84" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D84" s="23"/>
       <c r="E84" s="23" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F84" s="22"/>
     </row>
@@ -2855,14 +2855,14 @@
         <v>72</v>
       </c>
       <c r="B85" s="14" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C85" s="14" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D85" s="23"/>
       <c r="E85" s="23" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="F85" s="22"/>
     </row>
@@ -2871,14 +2871,14 @@
         <v>72</v>
       </c>
       <c r="B86" s="14" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C86" s="14" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D86" s="23"/>
       <c r="E86" s="23" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F86" s="22"/>
     </row>
@@ -2887,14 +2887,14 @@
         <v>72</v>
       </c>
       <c r="B87" s="14" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C87" s="14" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D87" s="23"/>
       <c r="E87" s="23" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="F87" s="22"/>
     </row>
@@ -2903,14 +2903,14 @@
         <v>72</v>
       </c>
       <c r="B88" s="14" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C88" s="14" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D88" s="23"/>
       <c r="E88" s="23" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F88" s="22"/>
     </row>
@@ -2919,14 +2919,14 @@
         <v>72</v>
       </c>
       <c r="B89" s="14" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C89" s="14" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D89" s="23"/>
       <c r="E89" s="23" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F89" s="22"/>
     </row>
@@ -2935,14 +2935,14 @@
         <v>72</v>
       </c>
       <c r="B90" s="14" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C90" s="14" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D90" s="23"/>
       <c r="E90" s="23" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F90" s="22"/>
     </row>
@@ -2951,14 +2951,14 @@
         <v>72</v>
       </c>
       <c r="B91" s="14" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C91" s="14" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D91" s="23"/>
       <c r="E91" s="23" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F91" s="22"/>
     </row>
@@ -2967,14 +2967,14 @@
         <v>72</v>
       </c>
       <c r="B92" s="14" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C92" s="14" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D92" s="23"/>
       <c r="E92" s="23" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F92" s="22"/>
     </row>
@@ -2983,14 +2983,14 @@
         <v>72</v>
       </c>
       <c r="B93" s="14" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C93" s="14" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D93" s="23"/>
       <c r="E93" s="23" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F93" s="22"/>
     </row>
@@ -2999,14 +2999,14 @@
         <v>72</v>
       </c>
       <c r="B94" s="14" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C94" s="14" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D94" s="23"/>
       <c r="E94" s="23" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F94" s="22"/>
     </row>
@@ -3015,14 +3015,14 @@
         <v>72</v>
       </c>
       <c r="B95" s="14" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C95" s="14" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D95" s="23"/>
       <c r="E95" s="23" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F95" s="22"/>
     </row>
@@ -3031,14 +3031,14 @@
         <v>72</v>
       </c>
       <c r="B96" s="14" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C96" s="14" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D96" s="23"/>
       <c r="E96" s="23" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F96" s="22"/>
     </row>
@@ -3047,14 +3047,14 @@
         <v>72</v>
       </c>
       <c r="B97" s="14" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C97" s="14" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D97" s="23"/>
       <c r="E97" s="23" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="F97" s="22"/>
     </row>
@@ -3063,14 +3063,14 @@
         <v>72</v>
       </c>
       <c r="B98" s="14" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C98" s="14" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D98" s="23"/>
       <c r="E98" s="23" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F98" s="22"/>
     </row>
@@ -3079,14 +3079,14 @@
         <v>72</v>
       </c>
       <c r="B99" s="14" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C99" s="14" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D99" s="23"/>
       <c r="E99" s="23" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F99" s="22"/>
     </row>
@@ -3095,14 +3095,14 @@
         <v>72</v>
       </c>
       <c r="B100" s="14" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C100" s="14" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D100" s="23"/>
       <c r="E100" s="23" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="F100" s="22"/>
     </row>
@@ -3111,14 +3111,14 @@
         <v>72</v>
       </c>
       <c r="B101" s="14" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C101" s="14" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D101" s="23"/>
       <c r="E101" s="23" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F101" s="22"/>
     </row>
@@ -3127,14 +3127,14 @@
         <v>72</v>
       </c>
       <c r="B102" s="14" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C102" s="14" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D102" s="23"/>
       <c r="E102" s="23" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F102" s="22"/>
     </row>
@@ -3143,14 +3143,14 @@
         <v>72</v>
       </c>
       <c r="B103" s="14" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C103" s="14" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D103" s="23"/>
       <c r="E103" s="23" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F103" s="22"/>
     </row>
@@ -3159,14 +3159,14 @@
         <v>72</v>
       </c>
       <c r="B104" s="14" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C104" s="14" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D104" s="23"/>
       <c r="E104" s="23" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F104" s="22"/>
     </row>
@@ -3191,14 +3191,14 @@
         <v>72</v>
       </c>
       <c r="B106" s="14" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C106" s="14" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D106" s="23"/>
       <c r="E106" s="23" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F106" s="22"/>
     </row>
@@ -3207,14 +3207,14 @@
         <v>72</v>
       </c>
       <c r="B107" s="14" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C107" s="14" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D107" s="23"/>
       <c r="E107" s="23" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F107" s="22"/>
     </row>
@@ -3223,14 +3223,14 @@
         <v>72</v>
       </c>
       <c r="B108" s="14" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C108" s="14" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D108" s="23"/>
       <c r="E108" s="23" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F108" s="22"/>
     </row>
@@ -3239,14 +3239,14 @@
         <v>72</v>
       </c>
       <c r="B109" s="14" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C109" s="14" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D109" s="23"/>
       <c r="E109" s="23" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F109" s="22"/>
     </row>
@@ -3255,14 +3255,14 @@
         <v>72</v>
       </c>
       <c r="B110" s="14" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C110" s="14" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D110" s="23"/>
       <c r="E110" s="23" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F110" s="22"/>
     </row>
@@ -3271,14 +3271,14 @@
         <v>72</v>
       </c>
       <c r="B111" s="14" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C111" s="14" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D111" s="23"/>
       <c r="E111" s="23" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F111" s="22"/>
     </row>
@@ -3303,14 +3303,14 @@
         <v>72</v>
       </c>
       <c r="B113" s="14" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C113" s="14" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D113" s="23"/>
       <c r="E113" s="23" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F113" s="22"/>
     </row>
@@ -3335,14 +3335,14 @@
         <v>72</v>
       </c>
       <c r="B115" s="14" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C115" s="14" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D115" s="23"/>
       <c r="E115" s="23" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F115" s="22"/>
     </row>
@@ -3351,14 +3351,14 @@
         <v>72</v>
       </c>
       <c r="B116" s="14" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C116" s="14" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D116" s="23"/>
       <c r="E116" s="23" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="F116" s="22"/>
     </row>
@@ -3367,14 +3367,14 @@
         <v>72</v>
       </c>
       <c r="B117" s="14" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C117" s="14" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D117" s="23"/>
       <c r="E117" s="23" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="F117" s="22"/>
     </row>
@@ -3383,14 +3383,14 @@
         <v>72</v>
       </c>
       <c r="B118" s="14" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C118" s="14" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D118" s="23"/>
       <c r="E118" s="23" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F118" s="22"/>
     </row>
@@ -3399,14 +3399,14 @@
         <v>72</v>
       </c>
       <c r="B119" s="14" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C119" s="14" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D119" s="23"/>
       <c r="E119" s="23" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F119" s="22"/>
     </row>
@@ -3415,14 +3415,14 @@
         <v>72</v>
       </c>
       <c r="B120" s="14" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C120" s="14" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D120" s="23"/>
       <c r="E120" s="23" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F120" s="22"/>
     </row>
@@ -3431,14 +3431,14 @@
         <v>72</v>
       </c>
       <c r="B121" s="14" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C121" s="14" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D121" s="23"/>
       <c r="E121" s="23" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F121" s="22"/>
     </row>
@@ -3447,14 +3447,14 @@
         <v>72</v>
       </c>
       <c r="B122" s="14" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C122" s="14" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D122" s="23"/>
       <c r="E122" s="23" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F122" s="22"/>
     </row>
@@ -3463,14 +3463,14 @@
         <v>72</v>
       </c>
       <c r="B123" s="14" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C123" s="14" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D123" s="23"/>
       <c r="E123" s="23" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F123" s="22"/>
     </row>
@@ -3479,14 +3479,14 @@
         <v>72</v>
       </c>
       <c r="B124" s="14" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C124" s="14" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D124" s="23"/>
       <c r="E124" s="23" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="F124" s="22"/>
     </row>
@@ -3495,14 +3495,14 @@
         <v>72</v>
       </c>
       <c r="B125" s="14" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C125" s="14" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D125" s="23"/>
       <c r="E125" s="23" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F125" s="22"/>
     </row>
@@ -3511,14 +3511,14 @@
         <v>72</v>
       </c>
       <c r="B126" s="14" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C126" s="14" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D126" s="23"/>
       <c r="E126" s="23" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="F126" s="22"/>
     </row>
@@ -3527,14 +3527,14 @@
         <v>72</v>
       </c>
       <c r="B127" s="14" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C127" s="14" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D127" s="23"/>
       <c r="E127" s="23" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F127" s="22"/>
     </row>
@@ -3543,14 +3543,14 @@
         <v>72</v>
       </c>
       <c r="B128" s="14" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C128" s="14" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D128" s="23"/>
       <c r="E128" s="23" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="F128" s="22"/>
     </row>
@@ -3559,14 +3559,14 @@
         <v>72</v>
       </c>
       <c r="B129" s="14" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C129" s="14" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D129" s="23"/>
       <c r="E129" s="23" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F129" s="22"/>
     </row>
@@ -3575,14 +3575,14 @@
         <v>72</v>
       </c>
       <c r="B130" s="14" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C130" s="14" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D130" s="23"/>
       <c r="E130" s="23" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F130" s="22"/>
     </row>
@@ -3591,14 +3591,14 @@
         <v>72</v>
       </c>
       <c r="B131" s="14" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C131" s="14" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D131" s="23"/>
       <c r="E131" s="23" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F131" s="22"/>
     </row>
@@ -3607,14 +3607,14 @@
         <v>72</v>
       </c>
       <c r="B132" s="14" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C132" s="14" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D132" s="23"/>
       <c r="E132" s="23" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F132" s="22"/>
     </row>
@@ -3623,14 +3623,14 @@
         <v>72</v>
       </c>
       <c r="B133" s="14" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C133" s="14" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D133" s="23"/>
       <c r="E133" s="23" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="F133" s="22"/>
     </row>
@@ -3639,14 +3639,14 @@
         <v>72</v>
       </c>
       <c r="B134" s="14" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C134" s="14" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D134" s="23"/>
       <c r="E134" s="23" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F134" s="22"/>
     </row>
@@ -3655,14 +3655,14 @@
         <v>72</v>
       </c>
       <c r="B135" s="14" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C135" s="14" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D135" s="23"/>
       <c r="E135" s="23" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="F135" s="22"/>
     </row>
@@ -3671,14 +3671,14 @@
         <v>72</v>
       </c>
       <c r="B136" s="14" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C136" s="14" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D136" s="23"/>
       <c r="E136" s="23" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="F136" s="22"/>
     </row>
@@ -3687,14 +3687,14 @@
         <v>72</v>
       </c>
       <c r="B137" s="14" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C137" s="14" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D137" s="23"/>
       <c r="E137" s="23" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F137" s="22"/>
     </row>
@@ -3703,14 +3703,14 @@
         <v>72</v>
       </c>
       <c r="B138" s="14" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C138" s="14" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D138" s="23"/>
       <c r="E138" s="23" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F138" s="22"/>
     </row>
@@ -3719,14 +3719,14 @@
         <v>72</v>
       </c>
       <c r="B139" s="14" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C139" s="14" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D139" s="23"/>
       <c r="E139" s="23" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="F139" s="22"/>
     </row>
@@ -3735,14 +3735,14 @@
         <v>72</v>
       </c>
       <c r="B140" s="14" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C140" s="14" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D140" s="23"/>
       <c r="E140" s="23" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="F140" s="22"/>
     </row>
@@ -3751,14 +3751,14 @@
         <v>72</v>
       </c>
       <c r="B141" s="14" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C141" s="14" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D141" s="23"/>
       <c r="E141" s="23" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F141" s="22"/>
     </row>
@@ -3767,14 +3767,14 @@
         <v>72</v>
       </c>
       <c r="B142" s="14" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C142" s="14" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D142" s="23"/>
       <c r="E142" s="23" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F142" s="22"/>
     </row>
@@ -3783,14 +3783,14 @@
         <v>72</v>
       </c>
       <c r="B143" s="14" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C143" s="14" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D143" s="23"/>
       <c r="E143" s="23" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F143" s="22"/>
     </row>
@@ -3799,14 +3799,14 @@
         <v>72</v>
       </c>
       <c r="B144" s="14" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C144" s="14" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D144" s="23"/>
       <c r="E144" s="23" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="F144" s="22"/>
     </row>
@@ -3815,14 +3815,14 @@
         <v>72</v>
       </c>
       <c r="B145" s="14" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C145" s="14" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D145" s="23"/>
       <c r="E145" s="23" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F145" s="22"/>
     </row>
@@ -3831,14 +3831,14 @@
         <v>72</v>
       </c>
       <c r="B146" s="14" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C146" s="14" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D146" s="23"/>
       <c r="E146" s="23" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="F146" s="22"/>
     </row>
@@ -3847,14 +3847,14 @@
         <v>72</v>
       </c>
       <c r="B147" s="14" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C147" s="14" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D147" s="23"/>
       <c r="E147" s="23" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F147" s="22"/>
     </row>
@@ -3863,14 +3863,14 @@
         <v>72</v>
       </c>
       <c r="B148" s="14" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C148" s="14" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D148" s="23"/>
       <c r="E148" s="23" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F148" s="22"/>
     </row>
@@ -3879,14 +3879,14 @@
         <v>72</v>
       </c>
       <c r="B149" s="14" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C149" s="14" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D149" s="23"/>
       <c r="E149" s="23" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F149" s="22"/>
     </row>
@@ -3895,14 +3895,14 @@
         <v>72</v>
       </c>
       <c r="B150" s="14" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C150" s="14" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D150" s="23"/>
       <c r="E150" s="23" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="F150" s="22"/>
     </row>
@@ -3919,7 +3919,7 @@
       <c r="D151" s="22"/>
       <c r="E151" s="22"/>
       <c r="F151" s="23" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.25">
@@ -3935,7 +3935,7 @@
       <c r="D152" s="22"/>
       <c r="E152" s="22"/>
       <c r="F152" s="23" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.25">
@@ -3951,7 +3951,7 @@
       <c r="D153" s="22"/>
       <c r="E153" s="22"/>
       <c r="F153" s="23" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.25">
@@ -3967,7 +3967,7 @@
       <c r="D154" s="22"/>
       <c r="E154" s="22"/>
       <c r="F154" s="23" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.25">
@@ -3983,7 +3983,7 @@
       <c r="D155" s="22"/>
       <c r="E155" s="22"/>
       <c r="F155" s="23" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.25">
@@ -3999,7 +3999,7 @@
       <c r="D156" s="22"/>
       <c r="E156" s="22"/>
       <c r="F156" s="23" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.25">
@@ -4015,7 +4015,7 @@
       <c r="D157" s="22"/>
       <c r="E157" s="22"/>
       <c r="F157" s="23" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.25">
@@ -4031,7 +4031,7 @@
       <c r="D158" s="22"/>
       <c r="E158" s="22"/>
       <c r="F158" s="23" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.25">
@@ -4047,7 +4047,7 @@
       <c r="D159" s="22"/>
       <c r="E159" s="22"/>
       <c r="F159" s="23" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.25">
@@ -4063,7 +4063,7 @@
       <c r="D160" s="22"/>
       <c r="E160" s="22"/>
       <c r="F160" s="23" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="161" spans="1:6" x14ac:dyDescent="0.25">
@@ -4079,7 +4079,7 @@
       <c r="D161" s="22"/>
       <c r="E161" s="22"/>
       <c r="F161" s="23" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="162" spans="1:6" x14ac:dyDescent="0.25">
@@ -4095,7 +4095,7 @@
       <c r="D162" s="22"/>
       <c r="E162" s="22"/>
       <c r="F162" s="23" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="163" spans="1:6" x14ac:dyDescent="0.25">
@@ -4111,7 +4111,7 @@
       <c r="D163" s="22"/>
       <c r="E163" s="22"/>
       <c r="F163" s="23" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="164" spans="1:6" x14ac:dyDescent="0.25">
@@ -4127,7 +4127,7 @@
       <c r="D164" s="22"/>
       <c r="E164" s="22"/>
       <c r="F164" s="23" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="165" spans="1:6" x14ac:dyDescent="0.25">
@@ -4143,7 +4143,7 @@
       <c r="D165" s="22"/>
       <c r="E165" s="22"/>
       <c r="F165" s="23" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="166" spans="1:6" x14ac:dyDescent="0.25">
@@ -4159,7 +4159,7 @@
       <c r="D166" s="22"/>
       <c r="E166" s="22"/>
       <c r="F166" s="23" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="167" spans="1:6" x14ac:dyDescent="0.25">
@@ -4175,7 +4175,7 @@
       <c r="D167" s="22"/>
       <c r="E167" s="22"/>
       <c r="F167" s="23" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="168" spans="1:6" x14ac:dyDescent="0.25">
@@ -4191,7 +4191,7 @@
       <c r="D168" s="22"/>
       <c r="E168" s="22"/>
       <c r="F168" s="23" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="169" spans="1:6" x14ac:dyDescent="0.25">
@@ -4207,7 +4207,7 @@
       <c r="D169" s="22"/>
       <c r="E169" s="22"/>
       <c r="F169" s="23" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="170" spans="1:6" x14ac:dyDescent="0.25">
@@ -4223,7 +4223,7 @@
       <c r="D170" s="22"/>
       <c r="E170" s="22"/>
       <c r="F170" s="23" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="171" spans="1:6" x14ac:dyDescent="0.25">
@@ -4239,7 +4239,7 @@
       <c r="D171" s="22"/>
       <c r="E171" s="22"/>
       <c r="F171" s="23" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="172" spans="1:6" x14ac:dyDescent="0.25">
@@ -4255,7 +4255,7 @@
       <c r="D172" s="22"/>
       <c r="E172" s="22"/>
       <c r="F172" s="23" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="173" spans="1:6" x14ac:dyDescent="0.25">
@@ -4271,7 +4271,7 @@
       <c r="D173" s="22"/>
       <c r="E173" s="22"/>
       <c r="F173" s="23" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="174" spans="1:6" x14ac:dyDescent="0.25">
@@ -4287,7 +4287,7 @@
       <c r="D174" s="22"/>
       <c r="E174" s="22"/>
       <c r="F174" s="23" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="175" spans="1:6" x14ac:dyDescent="0.25">
@@ -4303,7 +4303,7 @@
       <c r="D175" s="22"/>
       <c r="E175" s="22"/>
       <c r="F175" s="23" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="176" spans="1:6" x14ac:dyDescent="0.25">
@@ -4319,7 +4319,7 @@
       <c r="D176" s="22"/>
       <c r="E176" s="22"/>
       <c r="F176" s="23" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="177" spans="1:6" x14ac:dyDescent="0.25">
@@ -4335,7 +4335,7 @@
       <c r="D177" s="22"/>
       <c r="E177" s="22"/>
       <c r="F177" s="23" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="178" spans="1:6" x14ac:dyDescent="0.25">
@@ -4351,7 +4351,7 @@
       <c r="D178" s="22"/>
       <c r="E178" s="22"/>
       <c r="F178" s="23" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="179" spans="1:6" x14ac:dyDescent="0.25">
@@ -4367,7 +4367,7 @@
       <c r="D179" s="22"/>
       <c r="E179" s="22"/>
       <c r="F179" s="23" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="180" spans="1:6" x14ac:dyDescent="0.25">
@@ -4383,7 +4383,7 @@
       <c r="D180" s="22"/>
       <c r="E180" s="22"/>
       <c r="F180" s="23" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="181" spans="1:6" x14ac:dyDescent="0.25">
@@ -4399,7 +4399,7 @@
       <c r="D181" s="22"/>
       <c r="E181" s="22"/>
       <c r="F181" s="23" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="182" spans="1:6" x14ac:dyDescent="0.25">
@@ -4415,7 +4415,7 @@
       <c r="D182" s="22"/>
       <c r="E182" s="22"/>
       <c r="F182" s="23" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="183" spans="1:6" x14ac:dyDescent="0.25">
@@ -4431,7 +4431,7 @@
       <c r="D183" s="22"/>
       <c r="E183" s="22"/>
       <c r="F183" s="23" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="184" spans="1:6" x14ac:dyDescent="0.25">
@@ -4447,7 +4447,7 @@
       <c r="D184" s="22"/>
       <c r="E184" s="22"/>
       <c r="F184" s="23" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="185" spans="1:6" x14ac:dyDescent="0.25">
@@ -4463,7 +4463,7 @@
       <c r="D185" s="22"/>
       <c r="E185" s="22"/>
       <c r="F185" s="23" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="186" spans="1:6" x14ac:dyDescent="0.25">
@@ -4479,7 +4479,7 @@
       <c r="D186" s="22"/>
       <c r="E186" s="22"/>
       <c r="F186" s="23" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="187" spans="1:6" x14ac:dyDescent="0.25">
@@ -4495,7 +4495,7 @@
       <c r="D187" s="22"/>
       <c r="E187" s="22"/>
       <c r="F187" s="23" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="188" spans="1:6" x14ac:dyDescent="0.25">
@@ -4511,7 +4511,7 @@
       <c r="D188" s="22"/>
       <c r="E188" s="22"/>
       <c r="F188" s="23" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="189" spans="1:6" x14ac:dyDescent="0.25">
@@ -4527,7 +4527,7 @@
       <c r="D189" s="22"/>
       <c r="E189" s="22"/>
       <c r="F189" s="23" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="190" spans="1:6" x14ac:dyDescent="0.25">
@@ -4543,7 +4543,7 @@
       <c r="D190" s="22"/>
       <c r="E190" s="22"/>
       <c r="F190" s="23" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="191" spans="1:6" x14ac:dyDescent="0.25">
@@ -4559,7 +4559,7 @@
       <c r="D191" s="22"/>
       <c r="E191" s="22"/>
       <c r="F191" s="23" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="192" spans="1:6" x14ac:dyDescent="0.25">
@@ -4575,7 +4575,7 @@
       <c r="D192" s="22"/>
       <c r="E192" s="22"/>
       <c r="F192" s="23" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="193" spans="1:6" x14ac:dyDescent="0.25">
@@ -4591,7 +4591,7 @@
       <c r="D193" s="22"/>
       <c r="E193" s="22"/>
       <c r="F193" s="23" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="194" spans="1:6" x14ac:dyDescent="0.25">
@@ -4607,7 +4607,7 @@
       <c r="D194" s="22"/>
       <c r="E194" s="22"/>
       <c r="F194" s="23" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="195" spans="1:6" x14ac:dyDescent="0.25">
@@ -4623,7 +4623,7 @@
       <c r="D195" s="22"/>
       <c r="E195" s="22"/>
       <c r="F195" s="23" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="196" spans="1:6" x14ac:dyDescent="0.25">
@@ -4639,7 +4639,7 @@
       <c r="D196" s="22"/>
       <c r="E196" s="22"/>
       <c r="F196" s="23" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="197" spans="1:6" x14ac:dyDescent="0.25">
@@ -4655,7 +4655,7 @@
       <c r="D197" s="22"/>
       <c r="E197" s="22"/>
       <c r="F197" s="23" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="198" spans="1:6" x14ac:dyDescent="0.25">
@@ -4671,7 +4671,7 @@
       <c r="D198" s="22"/>
       <c r="E198" s="22"/>
       <c r="F198" s="23" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="199" spans="1:6" x14ac:dyDescent="0.25">
@@ -4687,7 +4687,7 @@
       <c r="D199" s="22"/>
       <c r="E199" s="22"/>
       <c r="F199" s="23" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="200" spans="1:6" x14ac:dyDescent="0.25">
@@ -4703,7 +4703,7 @@
       <c r="D200" s="22"/>
       <c r="E200" s="22"/>
       <c r="F200" s="23" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="201" spans="1:6" x14ac:dyDescent="0.25">
@@ -4719,7 +4719,7 @@
       <c r="D201" s="22"/>
       <c r="E201" s="22"/>
       <c r="F201" s="23" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="202" spans="1:6" x14ac:dyDescent="0.25">
@@ -4735,7 +4735,7 @@
       <c r="D202" s="22"/>
       <c r="E202" s="22"/>
       <c r="F202" s="23" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="203" spans="1:6" x14ac:dyDescent="0.25">
@@ -4751,7 +4751,7 @@
       <c r="D203" s="22"/>
       <c r="E203" s="22"/>
       <c r="F203" s="23" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="204" spans="1:6" x14ac:dyDescent="0.25">
@@ -4767,7 +4767,7 @@
       <c r="D204" s="22"/>
       <c r="E204" s="22"/>
       <c r="F204" s="23" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="205" spans="1:6" x14ac:dyDescent="0.25">
@@ -4783,7 +4783,7 @@
       <c r="D205" s="22"/>
       <c r="E205" s="22"/>
       <c r="F205" s="23" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="206" spans="1:6" x14ac:dyDescent="0.25">
@@ -4799,7 +4799,7 @@
       <c r="D206" s="22"/>
       <c r="E206" s="22"/>
       <c r="F206" s="23" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="207" spans="1:6" x14ac:dyDescent="0.25">
@@ -4815,7 +4815,7 @@
       <c r="D207" s="22"/>
       <c r="E207" s="22"/>
       <c r="F207" s="23" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="208" spans="1:6" x14ac:dyDescent="0.25">
@@ -4831,7 +4831,7 @@
       <c r="D208" s="22"/>
       <c r="E208" s="22"/>
       <c r="F208" s="23" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="209" spans="1:6" x14ac:dyDescent="0.25">
@@ -4847,7 +4847,7 @@
       <c r="D209" s="22"/>
       <c r="E209" s="22"/>
       <c r="F209" s="23" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="210" spans="1:6" x14ac:dyDescent="0.25">
@@ -4863,7 +4863,7 @@
       <c r="D210" s="22"/>
       <c r="E210" s="22"/>
       <c r="F210" s="23" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="211" spans="1:6" x14ac:dyDescent="0.25">
@@ -4879,7 +4879,7 @@
       <c r="D211" s="22"/>
       <c r="E211" s="22"/>
       <c r="F211" s="23" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="212" spans="1:6" x14ac:dyDescent="0.25">
@@ -4895,7 +4895,7 @@
       <c r="D212" s="22"/>
       <c r="E212" s="22"/>
       <c r="F212" s="23" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="213" spans="1:6" x14ac:dyDescent="0.25">
@@ -4911,7 +4911,7 @@
       <c r="D213" s="22"/>
       <c r="E213" s="22"/>
       <c r="F213" s="23" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="214" spans="1:6" x14ac:dyDescent="0.25">
@@ -4927,7 +4927,7 @@
       <c r="D214" s="22"/>
       <c r="E214" s="22"/>
       <c r="F214" s="23" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="215" spans="1:6" x14ac:dyDescent="0.25">
@@ -4991,7 +4991,7 @@
       <c r="D218" s="22"/>
       <c r="E218" s="22"/>
       <c r="F218" s="23" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="219" spans="1:6" x14ac:dyDescent="0.25">
@@ -5007,7 +5007,7 @@
       <c r="D219" s="22"/>
       <c r="E219" s="22"/>
       <c r="F219" s="23" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="220" spans="1:6" x14ac:dyDescent="0.25">
@@ -5023,7 +5023,7 @@
       <c r="D220" s="22"/>
       <c r="E220" s="22"/>
       <c r="F220" s="23" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="221" spans="1:6" x14ac:dyDescent="0.25">
@@ -5039,7 +5039,7 @@
       <c r="D221" s="22"/>
       <c r="E221" s="22"/>
       <c r="F221" s="23" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="222" spans="1:6" x14ac:dyDescent="0.25">
@@ -5055,7 +5055,7 @@
       <c r="D222" s="22"/>
       <c r="E222" s="22"/>
       <c r="F222" s="23" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="223" spans="1:6" x14ac:dyDescent="0.25">
@@ -5071,7 +5071,7 @@
       <c r="D223" s="22"/>
       <c r="E223" s="22"/>
       <c r="F223" s="23" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="224" spans="1:6" x14ac:dyDescent="0.25">
@@ -5087,7 +5087,7 @@
       <c r="D224" s="22"/>
       <c r="E224" s="22"/>
       <c r="F224" s="23" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="225" spans="1:6" x14ac:dyDescent="0.25">
@@ -5103,7 +5103,7 @@
       <c r="D225" s="22"/>
       <c r="E225" s="22"/>
       <c r="F225" s="23" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="226" spans="1:6" x14ac:dyDescent="0.25">
@@ -5119,7 +5119,7 @@
       <c r="D226" s="22"/>
       <c r="E226" s="22"/>
       <c r="F226" s="23" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="227" spans="1:6" x14ac:dyDescent="0.25">
@@ -5135,7 +5135,7 @@
       <c r="D227" s="22"/>
       <c r="E227" s="22"/>
       <c r="F227" s="23" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="228" spans="1:6" x14ac:dyDescent="0.25">
@@ -5151,7 +5151,7 @@
       <c r="D228" s="22"/>
       <c r="E228" s="22"/>
       <c r="F228" s="23" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="229" spans="1:6" x14ac:dyDescent="0.25">
@@ -5167,7 +5167,7 @@
       <c r="D229" s="22"/>
       <c r="E229" s="22"/>
       <c r="F229" s="23" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="230" spans="1:6" x14ac:dyDescent="0.25">
@@ -5183,7 +5183,7 @@
       <c r="D230" s="22"/>
       <c r="E230" s="22"/>
       <c r="F230" s="23" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="231" spans="1:6" x14ac:dyDescent="0.25">
@@ -5279,7 +5279,7 @@
       <c r="D236" s="22"/>
       <c r="E236" s="22"/>
       <c r="F236" s="23" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="237" spans="1:6" x14ac:dyDescent="0.25">
@@ -5295,7 +5295,7 @@
       <c r="D237" s="22"/>
       <c r="E237" s="22"/>
       <c r="F237" s="23" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="238" spans="1:6" x14ac:dyDescent="0.25">
@@ -5311,7 +5311,7 @@
       <c r="D238" s="22"/>
       <c r="E238" s="22"/>
       <c r="F238" s="23" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="239" spans="1:6" x14ac:dyDescent="0.25">
@@ -5327,7 +5327,7 @@
       <c r="D239" s="22"/>
       <c r="E239" s="22"/>
       <c r="F239" s="23" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="240" spans="1:6" x14ac:dyDescent="0.25">
@@ -5343,7 +5343,7 @@
       <c r="D240" s="22"/>
       <c r="E240" s="22"/>
       <c r="F240" s="23" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="241" spans="1:6" x14ac:dyDescent="0.25">
@@ -5359,7 +5359,7 @@
       <c r="D241" s="22"/>
       <c r="E241" s="22"/>
       <c r="F241" s="23" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="242" spans="1:6" x14ac:dyDescent="0.25">
@@ -5375,7 +5375,7 @@
       <c r="D242" s="22"/>
       <c r="E242" s="22"/>
       <c r="F242" s="23" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="243" spans="1:6" x14ac:dyDescent="0.25">
@@ -5391,7 +5391,7 @@
       <c r="D243" s="22"/>
       <c r="E243" s="22"/>
       <c r="F243" s="23" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="244" spans="1:6" x14ac:dyDescent="0.25">
@@ -5407,7 +5407,7 @@
       <c r="D244" s="22"/>
       <c r="E244" s="22"/>
       <c r="F244" s="23" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="245" spans="1:6" x14ac:dyDescent="0.25">
@@ -5423,7 +5423,7 @@
       <c r="D245" s="22"/>
       <c r="E245" s="22"/>
       <c r="F245" s="23" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="246" spans="1:6" x14ac:dyDescent="0.25">
@@ -5439,7 +5439,7 @@
       <c r="D246" s="22"/>
       <c r="E246" s="22"/>
       <c r="F246" s="23" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="247" spans="1:6" x14ac:dyDescent="0.25">
@@ -5455,7 +5455,7 @@
       <c r="D247" s="22"/>
       <c r="E247" s="22"/>
       <c r="F247" s="23" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="248" spans="1:6" x14ac:dyDescent="0.25">
@@ -5471,7 +5471,7 @@
       <c r="D248" s="22"/>
       <c r="E248" s="22"/>
       <c r="F248" s="23" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="249" spans="1:6" x14ac:dyDescent="0.25">
@@ -5487,7 +5487,7 @@
       <c r="D249" s="22"/>
       <c r="E249" s="22"/>
       <c r="F249" s="23" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="250" spans="1:6" x14ac:dyDescent="0.25">
@@ -5503,7 +5503,7 @@
       <c r="D250" s="22"/>
       <c r="E250" s="22"/>
       <c r="F250" s="23" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="251" spans="1:6" x14ac:dyDescent="0.25">
@@ -5519,7 +5519,7 @@
       <c r="D251" s="22"/>
       <c r="E251" s="22"/>
       <c r="F251" s="23" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="252" spans="1:6" x14ac:dyDescent="0.25">
@@ -5535,7 +5535,7 @@
       <c r="D252" s="22"/>
       <c r="E252" s="22"/>
       <c r="F252" s="23" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="253" spans="1:6" x14ac:dyDescent="0.25">
@@ -5583,7 +5583,7 @@
       <c r="D255" s="22"/>
       <c r="E255" s="22"/>
       <c r="F255" s="23" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="256" spans="1:6" x14ac:dyDescent="0.25">
@@ -5599,7 +5599,7 @@
       <c r="D256" s="22"/>
       <c r="E256" s="22"/>
       <c r="F256" s="23" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="257" spans="1:6" x14ac:dyDescent="0.25">
@@ -6000,8 +6000,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -6025,15 +6025,15 @@
         <v>13</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>89</v>
+        <v>225</v>
       </c>
       <c r="B2" t="s">
-        <v>88</v>
+        <v>224</v>
       </c>
       <c r="C2">
         <v>20201130</v>

</xml_diff>